<commit_message>
eooError added into core and updated
</commit_message>
<xml_diff>
--- a/speed test.xlsx
+++ b/speed test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\jm22kg\github\rCAT2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FC2CE00-C8D8-4AC9-91D3-E5D60E6D8111}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64E20ACA-B1BD-4EBE-A19E-7F767748B213}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="26">
   <si>
     <t>ahullmean</t>
   </si>
@@ -100,6 +100,9 @@
   </si>
   <si>
     <t>no</t>
+  </si>
+  <si>
+    <t>new speed</t>
   </si>
 </sst>
 </file>
@@ -440,18 +443,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>20</v>
@@ -459,8 +462,11 @@
       <c r="C1" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -474,7 +480,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -487,8 +493,11 @@
       <c r="D3" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -502,7 +511,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -516,7 +525,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -530,7 +539,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -544,7 +553,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -558,7 +567,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -572,7 +581,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -586,7 +595,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -600,7 +609,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -614,7 +623,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>13</v>
       </c>
@@ -628,7 +637,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -642,7 +651,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>16</v>
       </c>
@@ -656,7 +665,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -670,7 +679,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
         <v>0</v>
       </c>
@@ -684,7 +693,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
         <v>5</v>
       </c>
@@ -698,7 +707,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>15</v>
       </c>
@@ -712,7 +721,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>17</v>
       </c>
@@ -726,7 +735,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
         <v>18</v>
       </c>

</xml_diff>